<commit_message>
Update of local work on Shems Python.
</commit_message>
<xml_diff>
--- a/SHEMS python/single_building/results/profits.xlsx
+++ b/SHEMS python/single_building/results/profits.xlsx
@@ -473,7 +473,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>208.7295540998239</v>
+        <v>201.7009458245258</v>
       </c>
     </row>
     <row r="4">
@@ -503,7 +503,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>62.08071886198243</v>
+        <v>60.68899876601913</v>
       </c>
     </row>
     <row r="6">
@@ -563,7 +563,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>22.70983807868625</v>
+        <v>17.40995165602148</v>
       </c>
     </row>
     <row r="10">
@@ -593,7 +593,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>-88.9717318249958</v>
+        <v>-94.44648335722724</v>
       </c>
     </row>
     <row r="12">
@@ -608,7 +608,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>58.78878749917888</v>
+        <v>39.96873956131847</v>
       </c>
     </row>
     <row r="13">
@@ -623,7 +623,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>-60.02809503479193</v>
+        <v>-61.01363796799191</v>
       </c>
     </row>
     <row r="14">
@@ -653,7 +653,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>44.59809850901614</v>
+        <v>41.58579920735638</v>
       </c>
     </row>
     <row r="16">
@@ -668,7 +668,7 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>2.140679884847951</v>
+        <v>-10.48954692552599</v>
       </c>
     </row>
     <row r="17">
@@ -728,7 +728,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>-731.9087752897395</v>
+        <v>-733.8373775254573</v>
       </c>
     </row>
     <row r="21">
@@ -788,7 +788,7 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>-405.2767663701086</v>
+        <v>-414.9014438867886</v>
       </c>
     </row>
     <row r="25">
@@ -818,7 +818,7 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>-432.7142118875645</v>
+        <v>-444.4839643649241</v>
       </c>
     </row>
     <row r="27">
@@ -833,7 +833,7 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>-478.1943791456379</v>
+        <v>-514.3560478476167</v>
       </c>
     </row>
     <row r="28">
@@ -848,7 +848,7 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>-251.730020617484</v>
+        <v>-253.3854986589261</v>
       </c>
     </row>
     <row r="29">
@@ -863,7 +863,7 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>-457.6256161763106</v>
+        <v>-477.0838833015364</v>
       </c>
     </row>
     <row r="30">
@@ -908,7 +908,7 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>-369.5371911757879</v>
+        <v>-369.5371911757881</v>
       </c>
     </row>
   </sheetData>

</xml_diff>